<commit_message>
Fix job title lookup, add Chinese exclusion reasons, generate exclusion report
</commit_message>
<xml_diff>
--- a/筛选结果.xlsx
+++ b/筛选结果.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
@@ -1026,21 +1026,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PD134</t>
+          <t>PD133</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="n">
         <v>123</v>
       </c>
       <c r="D8" t="n">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>店2</t>
+          <t>店1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1055,15 +1055,19 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>兼职调茶大咖</t>
+          <t>店长</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2021-07-30</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
+          <t>2020-10-29</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2021-03-01</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
@@ -1082,22 +1086,18 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>2015-12-03</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
+          <t>2024-06-27</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="n">
-        <v>219.5</v>
+        <v>202</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>219.5</v>
+        <v>202</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1108,21 +1108,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PD135</t>
+          <t>PD134</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>123</v>
       </c>
       <c r="D9" t="n">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>店3</t>
+          <t>店2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1137,19 +1137,15 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>副经理</t>
+          <t>兼职调茶大咖</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2021-10-22</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2022-02-21</t>
-        </is>
-      </c>
+          <t>2021-07-30</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
@@ -1163,27 +1159,27 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>测试经理2</t>
+          <t>测试经理1</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>2015-12-24</t>
+          <t>2015-12-03</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>38.5</v>
+        <v>219.5</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>38.5</v>
+        <v>219.5</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1194,21 +1190,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PD141</t>
+          <t>PD135</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
         <v>123</v>
       </c>
       <c r="D10" t="n">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>店4</t>
+          <t>店3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1223,15 +1219,19 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>兼职调茶大咖</t>
+          <t>副经理</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2018-09-30</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
+          <t>2021-10-22</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2022-02-21</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
@@ -1250,18 +1250,22 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr"/>
+          <t>2015-12-24</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
       <c r="Q10" t="n">
-        <v>180</v>
+        <v>38.5</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>180</v>
+        <v>38.5</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1272,21 +1276,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PD142</t>
+          <t>PD141</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="n">
         <v>123</v>
       </c>
       <c r="D11" t="n">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>店5</t>
+          <t>店4</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1301,19 +1305,15 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>店长</t>
+          <t>兼职调茶大咖</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2020-08-21</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>2020-12-21</t>
-        </is>
-      </c>
+          <t>2018-09-30</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
@@ -1332,43 +1332,43 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>2016-07-01</t>
+          <t>2025-01-23</t>
         </is>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="R11" t="n">
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PD144</t>
+          <t>PD142</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
         <v>123</v>
       </c>
       <c r="D12" t="n">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>店2</t>
+          <t>店5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1383,17 +1383,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>副经理</t>
+          <t>店长</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2020-08-21</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2023-04-23</t>
+          <t>2020-12-21</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1409,52 +1409,48 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>测试经理1</t>
+          <t>测试经理2</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>2015-12-03</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr"/>
       <c r="Q12" t="n">
-        <v>5.5</v>
+        <v>116</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>5.5</v>
+        <v>116</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PD129</t>
+          <t>PD144</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C13" t="n">
         <v>123</v>
       </c>
       <c r="D13" t="n">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>店3</t>
+          <t>店2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1469,15 +1465,19 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>兼职调茶大咖</t>
+          <t>副经理</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2020-08-29</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2023-04-23</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
@@ -1491,27 +1491,27 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>测试经理2</t>
+          <t>测试经理1</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>2015-12-24</t>
+          <t>2015-12-03</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="R13" t="n">
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -1522,21 +1522,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PD153</t>
+          <t>PD129</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
         <v>123</v>
       </c>
       <c r="D14" t="n">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>店4</t>
+          <t>店3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2020-08-29</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1578,10 +1578,14 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr"/>
+          <t>2015-12-24</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
       <c r="Q14" t="n">
         <v>8</v>
       </c>
@@ -1600,21 +1604,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PD151</t>
+          <t>PD153</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" t="n">
         <v>123</v>
       </c>
       <c r="D15" t="n">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>店3</t>
+          <t>店4</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1629,19 +1633,15 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>副店长</t>
+          <t>兼职调茶大咖</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2022-02-09</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>2022-05-26</t>
-        </is>
-      </c>
+          <t>2024-04-03</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
@@ -1660,22 +1660,18 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>2015-12-24</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>2025-12-01</t>
-        </is>
-      </c>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
       <c r="Q15" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="R15" t="n">
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1686,21 +1682,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PD152</t>
+          <t>PD151</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="n">
         <v>123</v>
       </c>
       <c r="D16" t="n">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>店4</t>
+          <t>店3</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1715,17 +1711,17 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>店长</t>
+          <t>副店长</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2023-09-04</t>
+          <t>2022-02-09</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2023-12-29</t>
+          <t>2022-05-26</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1746,43 +1742,47 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr"/>
+          <t>2015-12-24</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
       <c r="Q16" t="n">
-        <v>23</v>
+        <v>9.5</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>23</v>
+        <v>9.5</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>否</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PD153</t>
+          <t>PD152</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="n">
         <v>123</v>
       </c>
       <c r="D17" t="n">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>店5</t>
+          <t>店4</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1797,15 +1797,19 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>兼职调茶大咖</t>
+          <t>店长</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
+          <t>2023-09-04</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2023-12-29</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
@@ -1824,18 +1828,18 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>2016-07-01</t>
+          <t>2025-01-23</t>
         </is>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -1846,21 +1850,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PD155</t>
+          <t>PD153</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" t="n">
         <v>123</v>
       </c>
       <c r="D18" t="n">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>店2</t>
+          <t>店5</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1880,7 +1884,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2021-12-07</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1897,27 +1901,23 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>测试经理1</t>
+          <t>测试经理2</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>2015-12-03</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PD156</t>
+          <t>PD155</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="n">
         <v>123</v>
       </c>
       <c r="D19" t="n">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>店3</t>
+          <t>店2</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2021-12-07</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1979,27 +1979,27 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>测试经理2</t>
+          <t>测试经理1</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>2015-12-24</t>
+          <t>2015-12-03</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -2010,11 +2010,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PD161</t>
+          <t>PD156</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" t="n">
         <v>123</v>
@@ -2039,19 +2039,15 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>副经理</t>
+          <t>兼职调茶大咖</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2020-09-19</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>2021-01-25</t>
-        </is>
-      </c>
+          <t>2023-02-15</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
@@ -2079,13 +2075,13 @@
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="R20" t="n">
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -2096,11 +2092,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PD132</t>
+          <t>PD142</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
         <v>123</v>
@@ -2125,15 +2121,19 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>兼职调茶大咖</t>
+          <t>店长</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2021-06-07</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+          <t>2020-08-21</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2020-12-21</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
@@ -2157,13 +2157,13 @@
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="R21" t="n">
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -2174,21 +2174,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PD167</t>
+          <t>PD161</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C22" t="n">
         <v>123</v>
       </c>
       <c r="D22" t="n">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>店1</t>
+          <t>店3</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2208,12 +2208,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2019-12-10</t>
+          <t>2020-09-19</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2020-05-26</t>
+          <t>2021-01-25</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2229,25 +2229,189 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>测试经理1</t>
+          <t>测试经理2</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>2024-06-27</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr"/>
+          <t>2015-12-24</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
       <c r="Q22" t="n">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="R22" t="n">
         <v>0</v>
       </c>
       <c r="S22" t="n">
+        <v>7</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PD132</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="n">
+        <v>123</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1125</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>店4</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>兼职调茶大咖</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2021-06-07</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>奈雪</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>测试区</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>测试经理2</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="n">
+        <v>9</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>9</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PD167</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>45</v>
+      </c>
+      <c r="C24" t="n">
+        <v>123</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1122</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>店1</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>副经理</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2019-12-10</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2020-05-26</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>奈雪</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>测试区</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>测试经理1</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>2024-06-27</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="n">
         <v>8.5</v>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="T24" t="inlineStr">
         <is>
           <t>否</t>
         </is>

</xml_diff>